<commit_message>
finished the Pandas project
</commit_message>
<xml_diff>
--- a/pandas_excel.xlsx
+++ b/pandas_excel.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>season</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>top_discipline</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>season</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -500,12 +500,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Taekwondo</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -537,12 +537,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -574,12 +574,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -611,12 +611,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>Weightlifting</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -648,12 +648,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>Swimming</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -685,12 +685,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Freestyle Skiing</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -722,12 +722,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>Handball</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -759,12 +759,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -796,12 +796,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>Wrestling Freestyle</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -833,12 +833,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -870,12 +870,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -907,12 +907,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -944,12 +944,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>Archery</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -981,12 +981,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>Bobsleigh</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1018,12 +1018,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1055,12 +1055,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>Biathlon</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1092,12 +1092,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1129,12 +1129,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1166,12 +1166,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1203,12 +1203,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
           <t>Weightlifting</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1240,12 +1240,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
           <t>Short Track Speed Skating</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1277,12 +1277,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
           <t>Rowing</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -1314,12 +1314,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
           <t>Ice Hockey</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1351,12 +1351,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -1388,12 +1388,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
           <t>Artistic G.</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -1425,12 +1425,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
           <t>Short Track Speed Skating</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -1462,12 +1462,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1499,12 +1499,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
           <t>Weightlifting</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -1573,12 +1573,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
           <t>Swimming</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -1610,12 +1610,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
           <t>Handball</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -1647,12 +1647,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -1684,12 +1684,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
           <t>Sailing</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -1721,12 +1721,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -1758,12 +1758,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
           <t>Ice Hockey</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -1795,12 +1795,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
           <t>Artistic G.</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -1832,12 +1832,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
           <t>Curling</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -1869,12 +1869,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -1906,12 +1906,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -1943,12 +1943,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -1980,12 +1980,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
           <t>Weightlifting</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -2017,12 +2017,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
           <t>Hockey</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -2054,12 +2054,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2091,12 +2091,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
           <t>Sailing</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -2128,12 +2128,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
           <t>Cross Country Skiing</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -2165,12 +2165,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -2202,12 +2202,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -2239,12 +2239,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
           <t>Ice Hockey</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -2276,12 +2276,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
           <t>Fencing</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -2313,12 +2313,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -2350,12 +2350,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
           <t>Taekwondo</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -2387,12 +2387,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -2424,12 +2424,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
           <t>Ice Hockey</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -2461,12 +2461,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
           <t>Judo</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -2498,12 +2498,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
           <t>Rowing</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -2535,12 +2535,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
           <t>Biathlon</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -2572,12 +2572,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -2609,12 +2609,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -2646,12 +2646,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -2683,12 +2683,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -2720,12 +2720,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -2757,12 +2757,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
           <t>Shooting</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -2794,12 +2794,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
           <t>Table Tennis</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -2831,12 +2831,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
           <t>Fencing</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -2868,12 +2868,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
           <t>Figure skating</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -2905,12 +2905,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
           <t>Badminton</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -2942,12 +2942,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
           <t>Hockey</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -2979,12 +2979,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -3016,12 +3016,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
           <t>Weightlifting</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -3053,12 +3053,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
           <t>Handball</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -3090,12 +3090,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
           <t>Judo</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -3127,12 +3127,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
           <t>Fencing</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -3164,12 +3164,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
           <t>Cross Country Skiing</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -3201,12 +3201,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -3238,12 +3238,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
           <t>Artistic G.</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -3275,12 +3275,12 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
           <t>Ski Jumping</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -3312,12 +3312,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -3349,12 +3349,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
           <t>Cross Country Skiing</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -3386,12 +3386,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -3423,12 +3423,12 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
           <t>Wrestling Gre-R</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -3460,12 +3460,12 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
           <t>Handball</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -3497,12 +3497,12 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
           <t>Short Track Speed Skating</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -3534,12 +3534,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
           <t>Jumping</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -3571,12 +3571,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
           <t>Shooting</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -3608,12 +3608,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -3645,12 +3645,12 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
           <t>Luge</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -3682,12 +3682,12 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
           <t>Wrestling Gre-R</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -3719,12 +3719,12 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
           <t>Basketball</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -3756,12 +3756,12 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -3793,12 +3793,12 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -3830,12 +3830,12 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -3867,12 +3867,12 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
           <t>Badminton</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -3904,12 +3904,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I94" t="n">
@@ -3941,12 +3941,12 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -3978,12 +3978,12 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
           <t>Wrestling Free.</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -4015,12 +4015,12 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
           <t>Wrestling Free.</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I97" t="n">
@@ -4052,12 +4052,12 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I98" t="n">
@@ -4089,12 +4089,12 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I99" t="n">
@@ -4126,12 +4126,12 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I100" t="n">
@@ -4163,12 +4163,12 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
           <t>Hockey</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I101" t="n">
@@ -4200,12 +4200,12 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
           <t>Speed skating</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I102" t="n">
@@ -4237,12 +4237,12 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I103" t="n">
@@ -4274,12 +4274,12 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I104" t="n">
@@ -4311,12 +4311,12 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
           <t>Sailing</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I105" t="n">
@@ -4348,12 +4348,12 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
           <t>Cross Country Skiing</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I106" t="n">
@@ -4385,12 +4385,12 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
           <t>Rowing</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I107" t="n">
@@ -4422,12 +4422,12 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I108" t="n">
@@ -4459,12 +4459,12 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
           <t>Hockey</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I109" t="n">
@@ -4496,12 +4496,12 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I110" t="n">
@@ -4533,12 +4533,12 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I111" t="n">
@@ -4570,12 +4570,12 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
           <t>Volleyball</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I112" t="n">
@@ -4607,12 +4607,12 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I113" t="n">
@@ -4644,12 +4644,12 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
           <t>Fencing</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I114" t="n">
@@ -4681,12 +4681,12 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
           <t>Speed skating</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I115" t="n">
@@ -4718,12 +4718,12 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I116" t="n">
@@ -4755,12 +4755,12 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I117" t="n">
@@ -4792,12 +4792,12 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I118" t="n">
@@ -4829,12 +4829,12 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I119" t="n">
@@ -4866,12 +4866,12 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
           <t>Biathlon</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I120" t="n">
@@ -4903,12 +4903,12 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
           <t>Water polo</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I121" t="n">
@@ -4940,12 +4940,12 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I122" t="n">
@@ -4977,12 +4977,12 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
           <t>Table Tennis</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I123" t="n">
@@ -5014,12 +5014,12 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
           <t>Rowing</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I124" t="n">
@@ -5051,12 +5051,12 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
           <t>Alpine Skiing</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I125" t="n">
@@ -5088,12 +5088,12 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H126" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I126" t="n">
@@ -5125,12 +5125,12 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I127" t="n">
@@ -5162,12 +5162,12 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
           <t>Artistic G.</t>
-        </is>
-      </c>
-      <c r="H128" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I128" t="n">
@@ -5199,12 +5199,12 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
           <t>Bobsleigh</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I129" t="n">
@@ -5236,12 +5236,12 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
           <t>Swimming</t>
-        </is>
-      </c>
-      <c r="H130" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I130" t="n">
@@ -5273,12 +5273,12 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
           <t>Canoe / Kayak S</t>
-        </is>
-      </c>
-      <c r="H131" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I131" t="n">
@@ -5310,12 +5310,12 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
           <t>Biathlon</t>
-        </is>
-      </c>
-      <c r="H132" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I132" t="n">
@@ -5347,12 +5347,12 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
           <t>Shooting</t>
-        </is>
-      </c>
-      <c r="H133" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I133" t="n">
@@ -5384,12 +5384,12 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
           <t>Ice Hockey</t>
-        </is>
-      </c>
-      <c r="H134" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I134" t="n">
@@ -5421,12 +5421,12 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I135" t="n">
@@ -5458,12 +5458,12 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H136" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I136" t="n">
@@ -5495,12 +5495,12 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H137" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I137" t="n">
@@ -5532,12 +5532,12 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H138" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I138" t="n">
@@ -5569,12 +5569,12 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
           <t>Canoe / Kayak S</t>
-        </is>
-      </c>
-      <c r="H139" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I139" t="n">
@@ -5606,12 +5606,12 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H140" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I140" t="n">
@@ -5643,12 +5643,12 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H141" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I141" t="n">
@@ -5680,12 +5680,12 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
           <t>Wrestling Free.</t>
-        </is>
-      </c>
-      <c r="H142" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I142" t="n">
@@ -5717,12 +5717,12 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
           <t>Shooting</t>
-        </is>
-      </c>
-      <c r="H143" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I143" t="n">
@@ -5754,12 +5754,12 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H144" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I144" t="n">
@@ -5791,12 +5791,12 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
           <t>Artistic G.</t>
-        </is>
-      </c>
-      <c r="H145" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I145" t="n">
@@ -5828,12 +5828,12 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
           <t>Biathlon</t>
-        </is>
-      </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I146" t="n">
@@ -5865,12 +5865,12 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
           <t>Football</t>
-        </is>
-      </c>
-      <c r="H147" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I147" t="n">
@@ -5902,12 +5902,12 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H148" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I148" t="n">
@@ -5939,12 +5939,12 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
           <t>Ice Hockey</t>
-        </is>
-      </c>
-      <c r="H149" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I149" t="n">
@@ -5976,12 +5976,12 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
           <t>Boxing</t>
-        </is>
-      </c>
-      <c r="H150" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I150" t="n">
@@ -6013,12 +6013,12 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
+          <t>winter</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
           <t>Freestyle Skiing</t>
-        </is>
-      </c>
-      <c r="H151" t="inlineStr">
-        <is>
-          <t>winter</t>
         </is>
       </c>
       <c r="I151" t="n">
@@ -6050,12 +6050,12 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
           <t>Taekwondo</t>
-        </is>
-      </c>
-      <c r="H152" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I152" t="n">
@@ -6087,12 +6087,12 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
           <t>Athletics</t>
-        </is>
-      </c>
-      <c r="H153" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I153" t="n">
@@ -6124,12 +6124,12 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
           <t>Hockey</t>
-        </is>
-      </c>
-      <c r="H154" t="inlineStr">
-        <is>
-          <t>summer</t>
         </is>
       </c>
       <c r="I154" t="n">

</xml_diff>